<commit_message>
Use 20-year financing repayment period and cite NREL ATB
</commit_message>
<xml_diff>
--- a/InputData/elec/RPfFESCC/RPfFESCC Repayment Period for Financed Elec Sector Capital Costs.xlsx
+++ b/InputData/elec/RPfFESCC/RPfFESCC Repayment Period for Financed Elec Sector Capital Costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\STfEPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\RPfFESCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45756452-2915-48CA-8D42-17979A9BDB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D36F59-E7C1-46A0-8442-832065985016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21705" yWindow="1950" windowWidth="33855" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21705" yWindow="1860" windowWidth="33855" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Source:</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>None needed</t>
-  </si>
-  <si>
     <t>RPfFESCC Repayment Period for Financed Electricity Sector Capital Costs</t>
   </si>
   <si>
@@ -62,6 +59,18 @@
   </si>
   <si>
     <t>Time Period</t>
+  </si>
+  <si>
+    <t>National Renewable Energy Laboratory</t>
+  </si>
+  <si>
+    <t>Annual Technology Baseline</t>
+  </si>
+  <si>
+    <t>https://atb.nrel.gov/electricity/2022/index</t>
+  </si>
+  <si>
+    <t>We use 20 years because this is the period used in NREL's Annual Electricity Technology Baseline.</t>
   </si>
 </sst>
 </file>
@@ -114,11 +123,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,16 +151,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -158,14 +168,19 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
@@ -446,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,77 +472,131 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="B4" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -535,11 +604,13 @@
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -547,27 +618,27 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,7 +646,7 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,9 +657,28 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{E264C0C9-8D50-4970-9ED0-F45FFE459EBD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -608,19 +698,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to 20 year repayment period to align with NREL ATB (Lazard also uses 20 years).
</commit_message>
<xml_diff>
--- a/InputData/elec/RPfFESCC/RPfFESCC Repayment Period for Financed Elec Sector Capital Costs.xlsx
+++ b/InputData/elec/RPfFESCC/RPfFESCC Repayment Period for Financed Elec Sector Capital Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\RPfFESCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RPfFESCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D36F59-E7C1-46A0-8442-832065985016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EC3107-A379-4815-A725-E40D4B74474C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21705" yWindow="1860" windowWidth="33855" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,10 @@
     <t>Annual Technology Baseline</t>
   </si>
   <si>
-    <t>https://atb.nrel.gov/electricity/2022/index</t>
-  </si>
-  <si>
-    <t>We use 20 years because this is the period used in NREL's Annual Electricity Technology Baseline.</t>
+    <t>We use 30 years because this is the default period used in NREL's Annual Electricity Technology Baseline.</t>
+  </si>
+  <si>
+    <t>https://atb.nrel.gov/electricity/2023/index</t>
   </si>
 </sst>
 </file>
@@ -157,24 +157,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
@@ -461,163 +456,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
-        <v>2022</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
@@ -626,7 +540,6 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,11 +547,11 @@
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +559,6 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +574,6 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +600,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -698,10 +609,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -709,7 +620,7 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>20</v>
       </c>
     </row>

</xml_diff>